<commit_message>
prueba en test bucle de clicks en next
</commit_message>
<xml_diff>
--- a/excel_data.xlsx
+++ b/excel_data.xlsx
@@ -440,35 +440,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Televisor Samsung Crystal 4K 60" UN60AU700...</t>
+          <t>Televisor PANASONIC LED 32'' HD Smart TV T...</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>S/. 2,499.00</t>
+          <t>S/. 899.00</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>S/2,299.00
--28%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>S/. 3,199.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG LED 43'' FHD Smart Tv UN...</t>
+          <t>Televisor Xiaomi Mi LED TV 4A 32' Smart HD...</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>S/. 1,499.00</t>
+          <t>S/. 989.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -485,35 +484,34 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG CRYSTAL UHD 55" Ultra HD...</t>
+          <t>Televisor HYUNDAI LED 58" UHD 4K Smart Tv ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S/. 1,999.00</t>
+          <t>S/. 1,899.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>S/1,899.00
--36%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>S/. 2,999.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Televisor LG UHD 4K ThinQ AI 50" 50UP7750 ...</t>
+          <t>Televisor LG HD ThinQ AI 32" 32LM637B</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>S/. 2,199.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -530,35 +528,34 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG CRYSTAL UHD 65" Ultra HD...</t>
+          <t>Televisor LG NanoCell 4K Procesador Inteli...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>S/. 2,799.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>S/2,599.00
--36%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>S/. 4,099.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Televisor LG LED 50'' UHD 4K Smart Tv 50UP...</t>
+          <t>Televisor LG NanoCell 4K ThinQ AI 70" 70NA...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>S/. 2,199.00</t>
+          <t>S/. 4,299.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -575,12 +572,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Televisor LG LED 65'' UHD 4K Smart Tv 65UP...</t>
+          <t>TV Smart LG 4K 75" NanoCell, Thinq Ai, Ult...</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>S/. 2,899.00</t>
+          <t>S/. 4,999.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -597,12 +594,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Televisor LG UHD 4K ThinQ AI 43" 43UP7700 ...</t>
+          <t>TELEVISOR LG 75" UHD 4K MOD: 75UP7750PSB</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>S/. 1,799.00</t>
+          <t>S/. 4,399.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -619,12 +616,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Televisor HISENSE LED 32'' HD Smart Tv 32A...</t>
+          <t>Xiaomi TV Smart 43" 4K UHD Modelo: L43M6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>S/. 749.00</t>
+          <t>S/. 1,499.00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -641,7 +638,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Televisor Samsung 50" AU7000 UHD 4K Smart ...</t>
+          <t>Televisor Hisense LED UHD 58" 58A6GSV</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -651,48 +648,46 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>S/1,799.00
--28%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>S/. 2,499.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Televisor Samsung AU7000 58" UHD 4K Smart ...</t>
+          <t>Televisor Hisense LED HD 32" 32A4GSV</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>S/. 2,399.00</t>
+          <t>S/. 749.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>S/2,199.00
--24%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>S/. 2,899.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG CRYSTAL UHD 65" Ultra HD...</t>
+          <t>Televisor Hisense LED UHD 50" 50A6GSV</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>S/. 3,449.00</t>
+          <t>S/. 1,499.00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -709,35 +704,34 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Televisor LG LED 55'' UHD 4K Smart Tv 55UP...</t>
+          <t>COMBO Televisor LG Smart TV UHD 55" + Máqu...</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>S/. 2,199.00</t>
+          <t>S/. 2,099.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>S/2,049.00
--24%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>S/. 2,699.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Televisor LG NanoCell 50'' 4K ThinQ AI 50N...</t>
+          <t>TV Smart Xiaomi Mi TV P1 32" LED, HD, sist...</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>S/. 2,399.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -754,12 +748,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Televisor LG LED 32" HD ThinQ AI 32LM637B</t>
+          <t>TV Smart Xiaomi Mi TV Q1 4K 75" QLED, Ultr...</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>S/. 1,149.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -776,12 +770,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Televisor HYUNDAI LED 42" FHD Smart TV HYL...</t>
+          <t>TV Smart Xiaomi Mi TV P1 4K 50" LED, Ultra...</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>S/. 1,199.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -798,7 +792,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Soporte Universal Móvil para TV 32"- 65" M...</t>
+          <t>TV Smart Xiaomi Mi TV P1 4K 55" LED, Ultra...</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -820,12 +814,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Televisor PHILIPS LED 50'' UHD 4K Smart Tv...</t>
+          <t>Soporte de Pared Fijo Inclinable para TV 3...</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>S/. 1,699.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -842,12 +836,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Televisor HISENSE LED 58'' UHD 4K Smart Tv...</t>
+          <t>Televisor LED SMART HD 32" 32S5195</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>S/. 1,699.00</t>
+          <t>S/. 949.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -864,12 +858,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Televisor LG UHD 43'' 4K ThinQ AI 43UP7700...</t>
+          <t>Televisor AOC LED SMART FHD 43" 43S5195</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>S/. 1,649.00</t>
+          <t>S/. 1,399.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -886,12 +880,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG LED 43" Ultra HD / 4K Sm...</t>
+          <t>TELEVISOR SAMSUNG 65" MOD: QN65Q70AAGXPE</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>S/. 1,799.00</t>
+          <t>S/. 5,179.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -908,12 +902,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG CRYSTAL UHD 55" Ultra HD...</t>
+          <t>TELEVISOR SAMSUNG 65" MOD: UN65AU8000GXPE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>S/. 2,449.00</t>
+          <t>S/. 3,579.00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -930,12 +924,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Televisor SAMSUNG CRYSTAL UHD 50" Ultra HD...</t>
+          <t>TELEVISOR SAMSUNG 55" MOD: UN55AU8000GXPE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>S/. 2,299.00</t>
+          <t>S/. 2,539.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -952,12 +946,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Televisor PHILIPS LED 32" HD Smart Tv 32PH...</t>
+          <t>TELEVISOR SAMSUNG 58" MOD: UN58AU7000GXPE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>S/. 849.00</t>
+          <t>S/. 2,539.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">

</xml_diff>

<commit_message>
ultima actualizacion save excel con 10 paginas de televisores prueba 2
</commit_message>
<xml_diff>
--- a/excel_data.xlsx
+++ b/excel_data.xlsx
@@ -446,7 +446,7 @@
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="65.85546875" customWidth="1" min="1" max="1"/>
     <col width="20.7109375" customWidth="1" min="2" max="2"/>
@@ -990,12 +990,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Televisor PANASONIC LED 32'' HD Smart TV T...</t>
+          <t>TELEVISOR SAMSUNG 55" MOD: UN55AU7000GXPE</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>S/. 899.00</t>
+          <t>S/. 2,279.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1012,12 +1012,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Televisor Xiaomi Mi LED TV 4A 32' Smart HD...</t>
+          <t>TELEVISOR SAMSUNG 50" MOD: UN50AU8000GXPE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>S/. 989.00</t>
+          <t>S/. 2,379.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1034,12 +1034,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Televisor HYUNDAI LED 58" UHD 4K Smart Tv ...</t>
+          <t>TELEVISOR SAMSUNG 50" MOD: UN50AU7000GXPE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>S/. 1,899.00</t>
+          <t>S/. 2,179.00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1056,12 +1056,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Televisor LG HD ThinQ AI 32" 32LM637B</t>
+          <t>TELEVISOR SAMSUNG 70" MOD: UN70AU7000GXPE</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 3,729.00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1078,12 +1078,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Televisor LG NanoCell 4K Procesador Inteli...</t>
+          <t>TELEVISOR SAMSUNG 65" MOD: UN65AU7000GXPE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 2,899.00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1100,12 +1100,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Televisor LG NanoCell 4K ThinQ AI 70" 70NA...</t>
+          <t>TELEVISOR SAMSUNG 50" MOD: QN50Q60AAGXPE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>S/. 4,299.00</t>
+          <t>S/. 2,589.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1122,12 +1122,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TV Smart LG 4K 75" NanoCell, Thinq Ai, Ult...</t>
+          <t>TELEVISOR SAMSUNG 43" MOD: UN43AU7000GXPE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>S/. 4,999.00</t>
+          <t>S/. 1,759.00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1144,12 +1144,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TELEVISOR LG 75" UHD 4K MOD: 75UP7750PSB</t>
+          <t>Amazon Fire TV Stick 4K Ultra HD con Alexa</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>S/. 4,399.00</t>
+          <t>S/. 299.00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1166,12 +1166,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Xiaomi TV Smart 43" 4K UHD Modelo: L43M6</t>
+          <t>Amazon Fire TV Stick 3ra Gen con Alexa Ful...</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>S/. 1,499.00</t>
+          <t>S/. 249.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1188,12 +1188,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Televisor Hisense LED UHD 58" 58A6GSV</t>
+          <t>Televisor Samsung Crystal UHD 60" UN60AU70...</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>S/. 1,899.00</t>
+          <t>S/. 2,499.00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1210,12 +1210,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Televisor Hisense LED HD 32" 32A4GSV</t>
+          <t>COMBO Televisor Crystal UHD 60" + Máquina ...</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>S/. 749.00</t>
+          <t>S/. 2,499.00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1232,12 +1232,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Televisor Hisense LED UHD 50" 50A6GSV</t>
+          <t>LG TV Smart 4K AI 55" Smart TV Procesad...</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>S/. 1,499.00</t>
+          <t>S/. 2,279.00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1254,12 +1254,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>COMBO Televisor LG Smart TV UHD 55" + Máqu...</t>
+          <t>LG TV 55UN711C 55?,4K Ultra HD Smart TV AI...</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>S/. 2,099.00</t>
+          <t>S/. 2,169.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1276,34 +1276,35 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TV Smart Xiaomi Mi TV P1 32" LED, HD, sist...</t>
+          <t>LG TV Smart 4K AI 50" Smart TV Procesad...</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 2,119.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/1,999.00
+-29%</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 2,799.00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TV Smart Xiaomi Mi TV Q1 4K 75" QLED, Ultr...</t>
+          <t>Televisor Samsung Smart TV 70" Q60A QLED 4...</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 5,399.00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1320,12 +1321,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TV Smart Xiaomi Mi TV P1 4K 50" LED, Ultra...</t>
+          <t>Televisor Samsung Smart TV 55" QLED 4K Q80...</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 3,899.00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1342,12 +1343,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TV Smart Xiaomi Mi TV P1 4K 55" LED, Ultra...</t>
+          <t>LG UHD AI ThinQ 55'' UP77 4K Smart Tv</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 2,398.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1364,12 +1365,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Soporte de Pared Fijo Inclinable para TV 3...</t>
+          <t>Televisor LG MINI LED 4K ThinQ AI 75" 75QN...</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>S/0</t>
+          <t>S/. 17,999.00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1386,12 +1387,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Televisor LED SMART HD 32" 32S5195</t>
+          <t>Televisor LG MINI LED 4K ThinQ AI 75" 75QN...</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>S/. 949.00</t>
+          <t>S/. 11,999.00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1408,12 +1409,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Televisor AOC LED SMART FHD 43" 43S5195</t>
+          <t>Televisor 43" LG UHD 4K</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>S/. 1,399.00</t>
+          <t>S/. 1,799.40</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1430,12 +1431,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 65" MOD: QN65Q70AAGXPE</t>
+          <t>LG UHD AI ThinQ 50'' UP77 4K Smart T</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>S/. 5,179.00</t>
+          <t>S/. 2,309.23</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1452,12 +1453,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 65" MOD: UN65AU8000GXPE</t>
+          <t>Televisor AOC LED 43" FHD Smart TV 43S5305</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>S/. 3,579.00</t>
+          <t>S/. 1,299.00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1474,12 +1475,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 55" MOD: UN55AU8000GXPE</t>
+          <t>Televisor PANASONIC LCD 43'' UHD 4K Smart ...</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>S/. 2,539.00</t>
+          <t>S/. 1,799.00</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1496,12 +1497,12 @@
     <row r="48" customFormat="1" s="2">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 58" MOD: UN58AU7000GXPE</t>
+          <t>Televisor SONY LCD 65'' Ultra HD / 4K Smar...</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>S/. 2,539.00</t>
+          <t>S/. 4,399.00</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
@@ -1518,12 +1519,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 55" MOD: UN55AU7000GXPE</t>
+          <t>Televisor LG OLED 65'' 4K ThinQ AI OLED65G...</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>S/. 2,279.00</t>
+          <t>S/. 9,999.00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1540,12 +1541,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 50" MOD: UN50AU8000GXPE</t>
+          <t>Televisor LG NanoCell 65'' UHD 4K ThinQ AI...</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>S/. 2,379.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1562,12 +1563,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 50" MOD: UN50AU7000GXPE</t>
+          <t>Televisor PANASONIC LCD 40'' HD Smart Tv T...</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>S/. 2,179.00</t>
+          <t>S/. 1,349.00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1584,12 +1585,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 70" MOD: UN70AU7000GXPE</t>
+          <t>Televisor HISENSE LED 65'' UHD 4K Smart TV...</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>S/. 3,729.00</t>
+          <t>S/. 2,199.00</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1606,12 +1607,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 65" MOD: UN65AU7000GXPE</t>
+          <t>Televisor HISENSE LED 50'' UHD 4K Smart TV...</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>S/. 2,899.00</t>
+          <t>S/. 1,499.00</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1628,12 +1629,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 50" MOD: QN50Q60AAGXPE</t>
+          <t>Televisor HISENSE LED 43'' FHD Smart Tv 43...</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>S/. 2,589.00</t>
+          <t>S/. 1,199.00</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1650,12 +1651,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TELEVISOR SAMSUNG 43" MOD: UN43AU7000GXPE</t>
+          <t>Televisor LG NanoCell 75'' UHD 4K ThinQ AI...</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>S/. 1,759.00</t>
+          <t>S/. 4,499.00</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1672,12 +1673,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Amazon Fire TV Stick 4K Ultra HD con Alexa</t>
+          <t>Televisor LG OLED 48'' 4K ThinQ AI OLED48A...</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>S/. 299.00</t>
+          <t>S/. 3,099.00</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1694,12 +1695,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Amazon Fire TV Stick 3ra Gen con Alexa Ful...</t>
+          <t>LG NanoCell 55'' NANO75 4K Smart TV</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>S/. 249.00</t>
+          <t>S/. 2,629.00</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1716,12 +1717,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Televisor Samsung Crystal UHD 60" UN60AU70...</t>
+          <t>LG OLED 65'' A1 4K Smart TV</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>S/. 2,499.00</t>
+          <t>S/. 6,879.00</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1738,12 +1739,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>COMBO Televisor Crystal UHD 60" + Máquina ...</t>
+          <t>LG OLED 65'' C1 4K Smart TV</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>S/. 2,499.00</t>
+          <t>S/. 7,589.00</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1760,12 +1761,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LG TV Smart 4K AI 55" Smart TV Procesad...</t>
+          <t>LG OLED 55'' A1 4K Smart TV con ThinQ AI, ...</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>S/. 2,279.00</t>
+          <t>S/. 4,299.00</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1782,12 +1783,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>LG TV 55UN711C 55?,4K Ultra HD Smart TV AI...</t>
+          <t>LG OLED 48'' A1 4K Smart TV con ThinQ A , ...</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>S/. 2,169.00</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1804,35 +1805,34 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LG TV Smart 4K AI 50" Smart TV Procesad...</t>
+          <t>Televisor Samsung Crystal UHD 50" UN50AU80...</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>S/. 2,119.00</t>
+          <t>S/. 2,299.00</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>S/1,999.00
--29%</t>
+          <t>S/0</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>S/. 2,799.00</t>
+          <t>S/0</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Televisor Samsung Smart TV 70" Q60A QLED 4...</t>
+          <t>COMBO Televisor UHD 65" + Máquina de pop c...</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>S/. 5,399.00</t>
+          <t>S/. 2,999.00</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1849,12 +1849,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Televisor Samsung Smart TV 55" QLED 4K Q80...</t>
+          <t>COMBO Televisor UHD 55" + Máquina de pop c...</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>S/. 3,899.00</t>
+          <t>S/. 2,199.00</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1871,12 +1871,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>LG UHD AI ThinQ 55'' UP77 4K Smart Tv</t>
+          <t>COMBO Televisor Qled 60" + Máquina de pop ...</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>S/. 2,398.00</t>
+          <t>S/. 3,249.00</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1893,12 +1893,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Televisor LG MINI LED 4K ThinQ AI 75" 75QN...</t>
+          <t>COMBO Televisor UHD 58" + Máquina de pop c...</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>S/. 17,999.00</t>
+          <t>S/. 2,449.00</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1915,12 +1915,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Televisor LG MINI LED 4K ThinQ AI 75" 75QN...</t>
+          <t>COMBO Televisor Crystal UHD 55" + Máquina ...</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>S/. 11,999.00</t>
+          <t>S/. 2,449.00</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1937,12 +1937,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Televisor 43" LG UHD 4K</t>
+          <t>COMBO Televisor UHD 50" + Máquina de pop c...</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>S/. 1,799.40</t>
+          <t>S/. 2,099.00</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1959,12 +1959,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>LG UHD AI ThinQ 50'' UP77 4K Smart T</t>
+          <t>COMBO Televisor Crystal UHD 50" + Máquina ...</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>S/. 2,309.23</t>
+          <t>S/. 2,299.00</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1981,12 +1981,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Televisor AOC LED 43" FHD Smart TV 43S5305</t>
+          <t>COMBO Televisor UHD 43" + Máquina de pop c...</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>S/. 1,299.00</t>
+          <t>S/. 1,799.00</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2003,12 +2003,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Televisor PANASONIC LCD 43'' UHD 4K Smart ...</t>
+          <t>COMBO Televisor Qled 65" + Máquina de pop ...</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>S/. 1,799.00</t>
+          <t>S/. 4,999.00</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2025,12 +2025,12 @@
     <row r="72" customFormat="1" s="2">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>Televisor SONY LCD 65'' Ultra HD / 4K Smar...</t>
+          <t>COMBO Televisor 50" + Máquina de pop corn</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>S/. 4,399.00</t>
+          <t>S/. 2,599.00</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">

</xml_diff>